<commit_message>
added handling of unassigned aps; leave excel old_site empty
</commit_message>
<xml_diff>
--- a/aps_serials.xlsx
+++ b/aps_serials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hpe-my.sharepoint.com/personal/andrew_lewandowski_hpe_com/Documents/Documents/python/pub_central_site_migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{9C5677F6-68CC-41B9-A2EA-EFDC1F1326B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83DFAAE4-62F5-4905-8E40-0D4FB06F9F3C}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{9C5677F6-68CC-41B9-A2EA-EFDC1F1326B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{497E058E-17B3-435B-9177-E7EBA02D0A76}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-96" windowWidth="30936" windowHeight="16896" xr2:uid="{58B93A9F-4B5E-4ED2-B76D-668DB22AA6C1}"/>
+    <workbookView xWindow="4560" yWindow="3564" windowWidth="17280" windowHeight="8964" xr2:uid="{58B93A9F-4B5E-4ED2-B76D-668DB22AA6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>CNPCKSM578</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>PHQFKYJ7J2</t>
-  </si>
-  <si>
-    <t>Test Site</t>
   </si>
   <si>
     <t>old_site</t>
@@ -441,7 +438,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,43 +451,34 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>